<commit_message>
Added tag distribution plots
</commit_message>
<xml_diff>
--- a/data_exploration/tag_stats/tag_stats_agglutinative.xlsx
+++ b/data_exploration/tag_stats/tag_stats_agglutinative.xlsx
@@ -84,10 +84,10 @@
     <t>O</t>
   </si>
   <si>
-    <t>DET</t>
+    <t>PART</t>
   </si>
   <si>
-    <t>PART</t>
+    <t>DET</t>
   </si>
   <si>
     <t>TRAIN</t>
@@ -122,7 +122,7 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -194,6 +194,264 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_finnish.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_basque.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_japanese.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_korean.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571525</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_turkish.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>742975</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>7</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="pos_tags_plot_agglutinative.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4000500"/>
+          <a:ext cx="12344425" cy="3429007"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1527,6 +1785,7 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2072,7 +2331,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>2428</v>
@@ -2084,7 +2343,7 @@
         <v>96.46723490558281</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12">
         <v>820</v>
@@ -2096,7 +2355,7 @@
         <v>96.43494500933804</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L12">
         <v>826</v>
@@ -2108,7 +2367,7 @@
         <v>96.27471896282924</v>
       </c>
       <c r="P12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q12">
         <v>4074</v>
@@ -2172,7 +2431,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>882</v>
@@ -2184,7 +2443,7 @@
         <v>99.19149286047085</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>292</v>
@@ -2196,7 +2455,7 @@
         <v>99.16165179497821</v>
       </c>
       <c r="K14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L14">
         <v>286</v>
@@ -2208,7 +2467,7 @@
         <v>99.10970706490522</v>
       </c>
       <c r="P14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q14">
         <v>1460</v>
@@ -2578,6 +2837,7 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3223,7 +3483,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>1058</v>
@@ -3235,7 +3495,7 @@
         <v>98.49834609092322</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <v>69</v>
@@ -3297,7 +3557,7 @@
         <v>99.19761766895526</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L15">
         <v>179</v>
@@ -3309,7 +3569,7 @@
         <v>99.07889317407421</v>
       </c>
       <c r="P15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q15">
         <v>1243</v>
@@ -3323,7 +3583,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>822</v>
@@ -3335,7 +3595,7 @@
         <v>99.56234102769254</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G16">
         <v>51</v>
@@ -3359,7 +3619,7 @@
         <v>99.56565694387238</v>
       </c>
       <c r="P16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q16">
         <v>1052</v>
@@ -3397,7 +3657,7 @@
         <v>100</v>
       </c>
       <c r="K17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L17">
         <v>116</v>
@@ -3435,7 +3695,7 @@
         <v>100</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -3447,7 +3707,7 @@
         <v>100</v>
       </c>
       <c r="K18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -3473,20 +3733,20 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>100</v>
+      </c>
+      <c r="F19" t="s">
         <v>20</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>100</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
       <c r="G19">
         <v>0</v>
       </c>
@@ -3497,7 +3757,7 @@
         <v>100</v>
       </c>
       <c r="K19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -3509,7 +3769,7 @@
         <v>100</v>
       </c>
       <c r="P19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -3523,7 +3783,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3535,7 +3795,7 @@
         <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3547,7 +3807,7 @@
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -3559,7 +3819,7 @@
         <v>100</v>
       </c>
       <c r="P20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -3573,7 +3833,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3585,7 +3845,7 @@
         <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -3597,7 +3857,7 @@
         <v>100</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -3609,7 +3869,7 @@
         <v>100</v>
       </c>
       <c r="P21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -3629,6 +3889,7 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4098,7 +4359,7 @@
         <v>92.10776169000712</v>
       </c>
       <c r="K10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L10">
         <v>496</v>
@@ -4148,7 +4409,7 @@
         <v>95.10641664688663</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L11">
         <v>465</v>
@@ -4224,7 +4485,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>4286</v>
@@ -4260,7 +4521,7 @@
         <v>99.22817173178967</v>
       </c>
       <c r="P13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q13">
         <v>5017</v>
@@ -4286,7 +4547,7 @@
         <v>99.25720029954864</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <v>266</v>
@@ -4398,7 +4659,7 @@
         <v>99.83384761452646</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -4410,7 +4671,7 @@
         <v>100</v>
       </c>
       <c r="P16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q16">
         <v>746</v>
@@ -4424,7 +4685,7 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>234</v>
@@ -4448,7 +4709,7 @@
         <v>99.91692380726323</v>
       </c>
       <c r="K17" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -4486,7 +4747,7 @@
         <v>99.98380818091658</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18">
         <v>16</v>
@@ -4498,7 +4759,7 @@
         <v>99.9802199541103</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -4598,7 +4859,7 @@
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -4648,7 +4909,7 @@
         <v>100</v>
       </c>
       <c r="K21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4680,6 +4941,7 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5149,7 +5411,7 @@
         <v>86.46944713870027</v>
       </c>
       <c r="K10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L10">
         <v>686</v>
@@ -5337,7 +5599,7 @@
         <v>98.14628353083936</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14">
         <v>191</v>
@@ -5361,7 +5623,7 @@
         <v>97.48796194233336</v>
       </c>
       <c r="P14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q14">
         <v>1523</v>
@@ -5375,7 +5637,7 @@
     </row>
     <row r="15" spans="1:19">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>646</v>
@@ -5575,7 +5837,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5587,7 +5849,7 @@
         <v>100</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -5625,7 +5887,7 @@
     </row>
     <row r="20" spans="1:19">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -5637,7 +5899,7 @@
         <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -5675,7 +5937,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -5687,7 +5949,7 @@
         <v>100</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -5699,7 +5961,7 @@
         <v>100</v>
       </c>
       <c r="K21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -5711,7 +5973,7 @@
         <v>100</v>
       </c>
       <c r="P21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -5731,6 +5993,7 @@
     <mergeCell ref="P1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6249,7 +6512,7 @@
         <v>97.39449821482847</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J14" s="1">
         <v>2.168562299792465</v>
@@ -6269,7 +6532,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1">
         <v>1.386326884413374</v>
@@ -6278,7 +6541,7 @@
         <v>98.74595858134708</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="1">
         <v>1.345987113533972</v>
@@ -6296,7 +6559,7 @@
         <v>98.31615941561529</v>
       </c>
       <c r="M15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N15" s="1">
         <v>1.529089432716923</v>
@@ -6325,7 +6588,7 @@
         <v>99.27223014677453</v>
       </c>
       <c r="I16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" s="1">
         <v>0.9197118135006004</v>
@@ -6345,7 +6608,7 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>0.3838588900674421</v>
@@ -6354,7 +6617,7 @@
         <v>99.64422271862732</v>
       </c>
       <c r="E17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F17" s="1">
         <v>0.3691865284317669</v>
@@ -6372,7 +6635,7 @@
         <v>99.65071857088989</v>
       </c>
       <c r="M17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N17" s="1">
         <v>0.4050608146804893</v>
@@ -6541,5 +6804,6 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>